<commit_message>
Reduce mo-cap length | Fix words size | Added trial lists files with practice field
</commit_message>
<xml_diff>
--- a/development/tests/practice_passed_tests.xlsx
+++ b/development/tests/practice_passed_tests.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA363B1-B256-4E0E-BAA9-5DAC94244AD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -101,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,7 +220,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -331,23 +329,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -383,23 +364,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -575,12 +539,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,12 +569,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -634,27 +598,27 @@
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -681,40 +645,40 @@
       <c r="B10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="20" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="11"/>

</xml_diff>